<commit_message>
New code is added
</commit_message>
<xml_diff>
--- a/src/main/java/com/cv/test/data/TestData.xlsx
+++ b/src/main/java/com/cv/test/data/TestData.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14520" windowHeight="4440"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14520" windowHeight="4365" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Exhibit" sheetId="2" r:id="rId2"/>
+    <sheet name="Sensor" sheetId="3" r:id="rId3"/>
+    <sheet name="Campaign" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:K13"/>
+  <oleSize ref="A1:M13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>Login</t>
   </si>
@@ -33,6 +36,81 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>Exhibit</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>VideoLink</t>
+  </si>
+  <si>
+    <t>SocialShareTitle</t>
+  </si>
+  <si>
+    <t>SocialShareDescription</t>
+  </si>
+  <si>
+    <t>BoothNumber</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>UUId</t>
+  </si>
+  <si>
+    <t>MajorId</t>
+  </si>
+  <si>
+    <t>MinorId</t>
+  </si>
+  <si>
+    <t>ModelVersion</t>
+  </si>
+  <si>
+    <t>FirmwareVersion</t>
+  </si>
+  <si>
+    <t>ManufactureName</t>
+  </si>
+  <si>
+    <t>testsen</t>
+  </si>
+  <si>
+    <t>NotificationText</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>Testcamp</t>
+  </si>
+  <si>
+    <t>nottitest</t>
+  </si>
+  <si>
+    <t>jh</t>
+  </si>
+  <si>
+    <t>CampaignName</t>
+  </si>
+  <si>
+    <t>Campaign</t>
   </si>
 </sst>
 </file>
@@ -382,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -437,4 +515,296 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="5" max="5" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>